<commit_message>
removed path line. adjusted y scale for even distribution. chart not displaying property feature unreadable for map
</commit_message>
<xml_diff>
--- a/data/Access_elec_HAP_CO2.xlsx
+++ b/data/Access_elec_HAP_CO2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="19760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,686 +686,686 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>24</v>
+        <v>736</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1">
-        <v>28.21566</v>
+        <v>22.615659999999998</v>
       </c>
       <c r="E2" s="1">
-        <v>31.05585</v>
+        <v>25.455850000000002</v>
       </c>
       <c r="F2" s="1">
-        <v>34.6</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1">
-        <v>37</v>
+        <v>32.562559999999998</v>
       </c>
       <c r="H2" s="4">
         <v>98</v>
       </c>
       <c r="I2" s="4">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="J2" s="4">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="K2" s="4">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="L2">
-        <v>-1.6599326446953E-2</v>
+        <v>-0.11851105026540799</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>48</v>
+        <v>894</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1">
-        <v>87.22775</v>
+        <v>13.33774</v>
       </c>
       <c r="E3" s="1">
-        <v>90.899180000000001</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F3" s="1">
-        <v>94.1</v>
+        <v>18.5</v>
       </c>
       <c r="G3" s="1">
-        <v>97.697829999999996</v>
+        <v>22.062560000000001</v>
       </c>
       <c r="H3" s="4">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="I3" s="4">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="J3" s="4">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="K3" s="4">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="L3">
-        <v>-3.46299068332563E-3</v>
+        <v>-7.0376415114256297E-2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>36.71566</v>
-      </c>
-      <c r="E4" s="1">
-        <v>39.555840000000003</v>
-      </c>
-      <c r="F4" s="1">
-        <v>43.1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>53.24</v>
-      </c>
-      <c r="H4" s="4">
-        <v>65</v>
-      </c>
-      <c r="I4" s="4">
-        <v>50</v>
-      </c>
-      <c r="J4" s="4">
-        <v>37</v>
-      </c>
-      <c r="K4" s="4">
-        <v>37</v>
-      </c>
-      <c r="L4">
-        <v>-1.7774428486346899E-2</v>
+      <c r="A4" s="2">
+        <v>320</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3">
+        <v>71.992450000000005</v>
+      </c>
+      <c r="E4" s="3">
+        <v>78</v>
+      </c>
+      <c r="F4" s="3">
+        <v>78.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>78.5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>64</v>
+      </c>
+      <c r="I4" s="5">
+        <v>59</v>
+      </c>
+      <c r="J4" s="5">
+        <v>57</v>
+      </c>
+      <c r="K4" s="5">
+        <v>64</v>
+      </c>
+      <c r="L4" s="2">
+        <v>-6.2630237324557997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>96</v>
+      <c r="A5">
+        <v>716</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3">
-        <v>65.691299999999998</v>
-      </c>
-      <c r="E5" s="3">
-        <v>69.362740000000002</v>
-      </c>
-      <c r="F5" s="3">
-        <v>72.599999999999994</v>
-      </c>
-      <c r="G5" s="3">
-        <v>76.161379999999994</v>
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="F5" s="1">
+        <v>36.9</v>
+      </c>
+      <c r="G5" s="1">
+        <v>40.462560000000003</v>
       </c>
       <c r="H5" s="4">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="I5" s="4">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="J5" s="4">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="K5" s="4">
-        <v>5</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1.08568847403414E-2</v>
+        <v>71</v>
+      </c>
+      <c r="L5">
+        <v>-5.6679640415408801E-2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>116</v>
+        <v>887</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1">
-        <v>19.237739999999999</v>
+        <v>38.459820000000001</v>
       </c>
       <c r="E6" s="1">
-        <v>16.600000000000001</v>
+        <v>41.3</v>
       </c>
       <c r="F6" s="1">
-        <v>31.1</v>
+        <v>44.8</v>
       </c>
       <c r="G6" s="1">
-        <v>31.1</v>
+        <v>48.406709999999997</v>
       </c>
       <c r="H6" s="4">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="J6" s="4">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="K6" s="4">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="L6">
-        <v>-1.83401260945402E-2</v>
+        <v>-3.6808169635344799E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>120</v>
+        <v>204</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>29</v>
+        <v>22.037739999999999</v>
       </c>
       <c r="E7" s="1">
-        <v>46.2</v>
+        <v>25.4</v>
       </c>
       <c r="F7" s="1">
-        <v>49</v>
+        <v>27.9</v>
       </c>
       <c r="G7" s="1">
-        <v>53.7</v>
+        <v>38.4</v>
       </c>
       <c r="H7" s="4">
+        <v>98</v>
+      </c>
+      <c r="I7" s="4">
         <v>94</v>
       </c>
-      <c r="I7" s="4">
-        <v>83</v>
-      </c>
       <c r="J7" s="4">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="K7" s="4">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="L7">
-        <v>0.29343089153145002</v>
+        <v>-2.3018394081025101E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>144</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>78.287729999999996</v>
+        <v>22.9</v>
       </c>
       <c r="E8" s="1">
-        <v>80.7</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="F8" s="1">
-        <v>85.1</v>
+        <v>32.5</v>
       </c>
       <c r="G8" s="1">
-        <v>88.662559999999999</v>
+        <v>36.076799999999999</v>
       </c>
       <c r="H8" s="4">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I8" s="4">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J8" s="4">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="K8" s="4">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="L8">
-        <v>-1.7264240988696299E-2</v>
+        <v>-2.16525842180945E-2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>170</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1">
-        <v>92</v>
+        <v>19.237739999999999</v>
       </c>
       <c r="E9" s="1">
-        <v>97</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="F9" s="1">
-        <v>96.7</v>
+        <v>31.1</v>
       </c>
       <c r="G9" s="1">
-        <v>97</v>
+        <v>31.1</v>
       </c>
       <c r="H9" s="4">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="I9" s="4">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="J9" s="4">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="K9" s="4">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="L9">
-        <v>-9.0146326877371605E-3</v>
+        <v>-1.83401260945402E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>178</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
-        <v>24.387740000000001</v>
+        <v>36.71566</v>
       </c>
       <c r="E10" s="1">
-        <v>20.9</v>
+        <v>39.555840000000003</v>
       </c>
       <c r="F10" s="1">
-        <v>37.1</v>
+        <v>43.1</v>
       </c>
       <c r="G10" s="1">
-        <v>41.6</v>
+        <v>53.24</v>
       </c>
       <c r="H10" s="4">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="I10" s="4">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="J10" s="4">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="K10" s="4">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="L10">
-        <v>0.75270354476254997</v>
+        <v>-1.7774428486346899E-2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1">
-        <v>6.3377400000000002</v>
+        <v>78.287729999999996</v>
       </c>
       <c r="E11" s="1">
-        <v>6.7</v>
+        <v>80.7</v>
       </c>
       <c r="F11" s="1">
-        <v>15.2</v>
+        <v>85.1</v>
       </c>
       <c r="G11" s="1">
-        <v>16.399999999999999</v>
+        <v>88.662559999999999</v>
       </c>
       <c r="H11" s="4">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I11" s="4">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="J11" s="4">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="K11" s="4">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="L11">
-        <v>0.118656743469492</v>
+        <v>-1.7264240988696299E-2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>204</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>22.037739999999999</v>
+        <v>28.21566</v>
       </c>
       <c r="E12" s="1">
-        <v>25.4</v>
+        <v>31.05585</v>
       </c>
       <c r="F12" s="1">
-        <v>27.9</v>
+        <v>34.6</v>
       </c>
       <c r="G12" s="1">
-        <v>38.4</v>
+        <v>37</v>
       </c>
       <c r="H12" s="4">
         <v>98</v>
       </c>
       <c r="I12" s="4">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="J12" s="4">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="K12" s="4">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="L12">
-        <v>-2.3018394081025101E-2</v>
+        <v>-1.6599326446953E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>218</v>
+        <v>686</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1">
-        <v>94</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="F13" s="1">
-        <v>97</v>
+        <v>56.5</v>
       </c>
       <c r="G13" s="1">
-        <v>97.2</v>
+        <v>56.5</v>
       </c>
       <c r="H13" s="4">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="I13" s="4">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="J13" s="4">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="K13" s="4">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="L13">
-        <v>-1.3942084392468E-3</v>
+        <v>-1.63205974174058E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>231</v>
+      <c r="A14" s="2">
+        <v>360</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="1">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1">
-        <v>12.7</v>
-      </c>
-      <c r="F14" s="1">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1">
-        <v>26.562560000000001</v>
+        <v>66</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3">
+        <v>66.86</v>
+      </c>
+      <c r="E14" s="3">
+        <v>87.6</v>
+      </c>
+      <c r="F14" s="3">
+        <v>94.2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>96</v>
       </c>
       <c r="H14" s="4">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="I14" s="4">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="J14" s="4">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="K14" s="4">
-        <v>95</v>
-      </c>
-      <c r="L14">
-        <v>8.1858143841486306E-2</v>
+        <v>39</v>
+      </c>
+      <c r="L14" s="2">
+        <v>-1.19737673603611E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>232</v>
+        <v>388</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1">
-        <v>22.9</v>
+        <v>85</v>
       </c>
       <c r="E15" s="1">
-        <v>32.200000000000003</v>
+        <v>86</v>
       </c>
       <c r="F15" s="1">
-        <v>32.5</v>
+        <v>92</v>
       </c>
       <c r="G15" s="1">
-        <v>36.076799999999999</v>
+        <v>92.633439999999993</v>
       </c>
       <c r="H15" s="4">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="I15" s="4">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="J15" s="4">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="K15" s="4">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="L15">
-        <v>-2.16525842180945E-2</v>
+        <v>-1.15492576293623E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>266</v>
+      <c r="A16" s="2">
+        <v>634</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1">
-        <v>72.987740000000002</v>
-      </c>
-      <c r="E16" s="1">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="F16" s="1">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="G16" s="1">
-        <v>89.3</v>
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3">
+        <v>87.22775</v>
+      </c>
+      <c r="E16" s="3">
+        <v>90.899180000000001</v>
+      </c>
+      <c r="F16" s="3">
+        <v>94.1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>97.697829999999996</v>
       </c>
       <c r="H16" s="4">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="I16" s="4">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J16" s="4">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="K16" s="4">
-        <v>20</v>
-      </c>
-      <c r="L16">
-        <v>3.50294896423341E-2</v>
+        <v>5</v>
+      </c>
+      <c r="L16" s="2">
+        <v>-1.0775372395563001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>288</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1">
-        <v>30.6</v>
+        <v>92</v>
       </c>
       <c r="E17" s="1">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="F17" s="1">
-        <v>60.5</v>
+        <v>96.7</v>
       </c>
       <c r="G17" s="1">
-        <v>64.062560000000005</v>
+        <v>97</v>
       </c>
       <c r="H17" s="4">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="I17" s="4">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="J17" s="4">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="K17" s="4">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="L17">
-        <v>1.80172553203303E-2</v>
+        <v>-9.0146326877371605E-3</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>320</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3">
-        <v>71.992450000000005</v>
-      </c>
-      <c r="E18" s="3">
-        <v>78</v>
-      </c>
-      <c r="F18" s="3">
-        <v>78.3</v>
-      </c>
-      <c r="G18" s="3">
-        <v>78.5</v>
-      </c>
-      <c r="H18" s="5">
-        <v>64</v>
-      </c>
-      <c r="I18" s="5">
-        <v>59</v>
-      </c>
-      <c r="J18" s="5">
-        <v>57</v>
-      </c>
-      <c r="K18" s="5">
-        <v>64</v>
-      </c>
-      <c r="L18" s="2">
-        <v>-6.2630237324557997E-2</v>
+      <c r="A18">
+        <v>682</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>87.22775</v>
+      </c>
+      <c r="E18" s="1">
+        <v>90.899180000000001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>94.1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>97.697829999999996</v>
+      </c>
+      <c r="H18" s="4">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5</v>
+      </c>
+      <c r="J18" s="4">
+        <v>5</v>
+      </c>
+      <c r="K18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>-7.3626702159709199E-3</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>332</v>
+      <c r="A19">
+        <v>760</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="3">
-        <v>31.3</v>
-      </c>
-      <c r="E19" s="3">
-        <v>31.4</v>
-      </c>
-      <c r="F19" s="3">
-        <v>33.9</v>
-      </c>
-      <c r="G19" s="3">
-        <v>37.9</v>
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1">
+        <v>85.037729999999996</v>
+      </c>
+      <c r="E19" s="1">
+        <v>86.6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>92.7</v>
+      </c>
+      <c r="G19" s="1">
+        <v>96.262559999999993</v>
       </c>
       <c r="H19" s="4">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="I19" s="4">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="J19" s="4">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="K19" s="4">
-        <v>92</v>
-      </c>
-      <c r="L19" s="2">
-        <v>3.5485968245378398E-2</v>
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>-5.7549555396940698E-3</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1407,649 +1407,649 @@
       </c>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>356</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="3">
-        <v>50.9</v>
-      </c>
-      <c r="E21" s="3">
-        <v>62.3</v>
-      </c>
-      <c r="F21" s="3">
-        <v>75</v>
-      </c>
-      <c r="G21" s="3">
-        <v>78.7</v>
-      </c>
-      <c r="H21" s="5">
-        <v>87</v>
-      </c>
-      <c r="I21" s="5">
-        <v>71</v>
-      </c>
-      <c r="J21" s="5">
-        <v>58</v>
-      </c>
-      <c r="K21" s="5">
-        <v>64</v>
-      </c>
-      <c r="L21" s="2">
-        <v>6.3566081806801303E-3</v>
+      <c r="A21">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>87.22775</v>
+      </c>
+      <c r="E21" s="1">
+        <v>90.899180000000001</v>
+      </c>
+      <c r="F21" s="1">
+        <v>94.1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>97.697829999999996</v>
+      </c>
+      <c r="H21" s="4">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4">
+        <v>5</v>
+      </c>
+      <c r="J21" s="4">
+        <v>5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>-3.46299068332563E-3</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>360</v>
+      <c r="A22">
+        <v>218</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="3">
-        <v>66.86</v>
-      </c>
-      <c r="E22" s="3">
-        <v>87.6</v>
-      </c>
-      <c r="F22" s="3">
-        <v>94.2</v>
-      </c>
-      <c r="G22" s="3">
-        <v>96</v>
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1">
+        <v>89</v>
+      </c>
+      <c r="E22" s="1">
+        <v>94</v>
+      </c>
+      <c r="F22" s="1">
+        <v>97</v>
+      </c>
+      <c r="G22" s="1">
+        <v>97.2</v>
       </c>
       <c r="H22" s="4">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="I22" s="4">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="J22" s="4">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="K22" s="4">
-        <v>39</v>
-      </c>
-      <c r="L22" s="2">
-        <v>-1.19737673603611E-2</v>
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>-1.3942084392468E-3</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>384</v>
+      <c r="A23">
+        <v>414</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="3">
-        <v>36.5</v>
-      </c>
-      <c r="E23" s="3">
-        <v>51.4</v>
-      </c>
-      <c r="F23" s="3">
-        <v>58.9</v>
-      </c>
-      <c r="G23" s="3">
-        <v>55.8</v>
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="1">
+        <v>87.22775</v>
+      </c>
+      <c r="E23" s="1">
+        <v>90.899180000000001</v>
+      </c>
+      <c r="F23" s="1">
+        <v>94.1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>97.697829999999996</v>
       </c>
       <c r="H23" s="4">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="I23" s="4">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="J23" s="4">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="K23" s="4">
-        <v>81</v>
-      </c>
-      <c r="L23" s="2">
-        <v>4.7078589973181904E-3</v>
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <v>6.8626280231910404E-4</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>388</v>
+        <v>748</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1">
-        <v>85</v>
+        <v>28.815660000000001</v>
       </c>
       <c r="E24" s="1">
-        <v>86</v>
+        <v>31.655850000000001</v>
       </c>
       <c r="F24" s="1">
-        <v>92</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="G24" s="1">
-        <v>92.633439999999993</v>
+        <v>42</v>
       </c>
       <c r="H24" s="4">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="I24" s="4">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="J24" s="4">
+        <v>55</v>
+      </c>
+      <c r="K24" s="4">
+        <v>61</v>
+      </c>
+      <c r="L24">
+        <v>1.17074193572516E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>608</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="E25" s="3">
+        <v>71.3</v>
+      </c>
+      <c r="F25" s="3">
+        <v>83.3</v>
+      </c>
+      <c r="G25" s="3">
+        <v>87.5</v>
+      </c>
+      <c r="H25" s="5">
+        <v>60</v>
+      </c>
+      <c r="I25" s="5">
+        <v>53</v>
+      </c>
+      <c r="J25" s="5">
+        <v>50</v>
+      </c>
+      <c r="K25" s="5">
+        <v>54</v>
+      </c>
+      <c r="L25" s="2">
+        <v>3.57435856211897E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>384</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="4">
-        <v>11</v>
-      </c>
-      <c r="L24">
-        <v>-1.15492576293623E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>404</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1">
-        <v>10.9</v>
-      </c>
-      <c r="E25" s="1">
-        <v>14.5</v>
-      </c>
-      <c r="F25" s="1">
-        <v>23</v>
-      </c>
-      <c r="G25" s="1">
-        <v>23</v>
-      </c>
-      <c r="H25" s="4">
-        <v>82</v>
-      </c>
-      <c r="I25" s="4">
-        <v>80</v>
-      </c>
-      <c r="J25" s="4">
-        <v>80</v>
-      </c>
-      <c r="K25" s="4">
-        <v>84</v>
-      </c>
-      <c r="L25">
-        <v>3.6270228264209101E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>414</v>
-      </c>
-      <c r="B26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1">
-        <v>87.22775</v>
-      </c>
-      <c r="E26" s="1">
-        <v>90.899180000000001</v>
-      </c>
-      <c r="F26" s="1">
-        <v>94.1</v>
-      </c>
-      <c r="G26" s="1">
-        <v>97.697829999999996</v>
+      <c r="D26" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="E26" s="3">
+        <v>51.4</v>
+      </c>
+      <c r="F26" s="3">
+        <v>58.9</v>
+      </c>
+      <c r="G26" s="3">
+        <v>55.8</v>
       </c>
       <c r="H26" s="4">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="I26" s="4">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="J26" s="4">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="K26" s="4">
-        <v>5</v>
-      </c>
-      <c r="L26">
-        <v>6.8626280231910404E-4</v>
+        <v>81</v>
+      </c>
+      <c r="L26" s="2">
+        <v>4.7078589973181904E-3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>591</v>
-      </c>
-      <c r="B27" t="s">
+        <v>356</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="3">
+        <v>50.9</v>
+      </c>
+      <c r="E27" s="3">
+        <v>62.3</v>
+      </c>
+      <c r="F27" s="3">
+        <v>75</v>
+      </c>
+      <c r="G27" s="3">
+        <v>78.7</v>
+      </c>
+      <c r="H27" s="5">
+        <v>87</v>
+      </c>
+      <c r="I27" s="5">
         <v>71</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="3">
-        <v>81.135729999999995</v>
-      </c>
-      <c r="E27" s="3">
-        <v>85.411199999999994</v>
-      </c>
-      <c r="F27" s="3">
-        <v>87.873279999999994</v>
-      </c>
-      <c r="G27" s="3">
-        <v>90.875439999999998</v>
-      </c>
-      <c r="H27" s="4">
-        <v>25</v>
-      </c>
-      <c r="I27" s="4">
-        <v>20</v>
-      </c>
-      <c r="J27" s="4">
-        <v>18</v>
-      </c>
-      <c r="K27" s="4">
-        <v>15</v>
+      <c r="J27" s="5">
+        <v>58</v>
+      </c>
+      <c r="K27" s="5">
+        <v>64</v>
       </c>
       <c r="L27" s="2">
-        <v>1.93498964059396E-2</v>
+        <v>6.3566081806801303E-3</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>604</v>
+        <v>710</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1">
-        <v>72.861500000000007</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="F28" s="1">
-        <v>85</v>
+        <v>82.7</v>
       </c>
       <c r="G28" s="1">
-        <v>91.2</v>
+        <v>85.4</v>
       </c>
       <c r="H28" s="4">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="I28" s="4">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J28" s="4">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="K28" s="4">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="L28">
-        <v>6.3265690772740704E-2</v>
+        <v>9.7989716756891106E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>608</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D29" s="3">
-        <v>65.400000000000006</v>
+        <v>65.691299999999998</v>
       </c>
       <c r="E29" s="3">
-        <v>71.3</v>
+        <v>69.362740000000002</v>
       </c>
       <c r="F29" s="3">
-        <v>83.3</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="G29" s="3">
-        <v>87.5</v>
-      </c>
-      <c r="H29" s="5">
-        <v>60</v>
-      </c>
-      <c r="I29" s="5">
-        <v>53</v>
-      </c>
-      <c r="J29" s="5">
-        <v>50</v>
-      </c>
-      <c r="K29" s="5">
-        <v>54</v>
+        <v>76.161379999999994</v>
+      </c>
+      <c r="H29" s="4">
+        <v>5</v>
+      </c>
+      <c r="I29" s="4">
+        <v>5</v>
+      </c>
+      <c r="J29" s="4">
+        <v>5</v>
+      </c>
+      <c r="K29" s="4">
+        <v>5</v>
       </c>
       <c r="L29" s="2">
-        <v>3.57435856211897E-3</v>
+        <v>1.08568847403414E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>634</v>
+      <c r="A30">
+        <v>288</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="3">
-        <v>87.22775</v>
-      </c>
-      <c r="E30" s="3">
-        <v>90.899180000000001</v>
-      </c>
-      <c r="F30" s="3">
-        <v>94.1</v>
-      </c>
-      <c r="G30" s="3">
-        <v>97.697829999999996</v>
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="E30" s="1">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1">
+        <v>60.5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>64.062560000000005</v>
       </c>
       <c r="H30" s="4">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="I30" s="4">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="J30" s="4">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="K30" s="4">
-        <v>5</v>
-      </c>
-      <c r="L30" s="2">
-        <v>-1.0775372395563001E-2</v>
+        <v>83</v>
+      </c>
+      <c r="L30">
+        <v>1.80172553203303E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>682</v>
+      <c r="A31" s="2">
+        <v>591</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="1">
-        <v>87.22775</v>
-      </c>
-      <c r="E31" s="1">
-        <v>90.899180000000001</v>
-      </c>
-      <c r="F31" s="1">
-        <v>94.1</v>
-      </c>
-      <c r="G31" s="1">
-        <v>97.697829999999996</v>
+        <v>71</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>81.135729999999995</v>
+      </c>
+      <c r="E31" s="3">
+        <v>85.411199999999994</v>
+      </c>
+      <c r="F31" s="3">
+        <v>87.873279999999994</v>
+      </c>
+      <c r="G31" s="3">
+        <v>90.875439999999998</v>
       </c>
       <c r="H31" s="4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I31" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J31" s="4">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="K31" s="4">
-        <v>5</v>
-      </c>
-      <c r="L31">
-        <v>-7.3626702159709199E-3</v>
+        <v>15</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1.93498964059396E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>686</v>
+        <v>266</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1">
+        <v>72.987740000000002</v>
+      </c>
+      <c r="E32" s="1">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="F32" s="1">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="G32" s="1">
+        <v>89.3</v>
+      </c>
+      <c r="H32" s="4">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4">
+        <v>28</v>
+      </c>
+      <c r="J32" s="4">
         <v>26</v>
       </c>
-      <c r="E32" s="1">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="F32" s="1">
-        <v>56.5</v>
-      </c>
-      <c r="G32" s="1">
-        <v>56.5</v>
-      </c>
-      <c r="H32" s="4">
-        <v>81</v>
-      </c>
-      <c r="I32" s="4">
-        <v>65</v>
-      </c>
-      <c r="J32" s="4">
-        <v>51</v>
-      </c>
       <c r="K32" s="4">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="L32">
-        <v>-1.63205974174058E-2</v>
+        <v>3.50294896423341E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>710</v>
+      <c r="A33" s="2">
+        <v>332</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="1">
-        <v>65</v>
-      </c>
-      <c r="E33" s="1">
-        <v>66.099999999999994</v>
-      </c>
-      <c r="F33" s="1">
-        <v>82.7</v>
-      </c>
-      <c r="G33" s="1">
-        <v>85.4</v>
+        <v>63</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="3">
+        <v>31.3</v>
+      </c>
+      <c r="E33" s="3">
+        <v>31.4</v>
+      </c>
+      <c r="F33" s="3">
+        <v>33.9</v>
+      </c>
+      <c r="G33" s="3">
+        <v>37.9</v>
       </c>
       <c r="H33" s="4">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="I33" s="4">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="J33" s="4">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="K33" s="4">
-        <v>12</v>
-      </c>
-      <c r="L33">
-        <v>9.7989716756891106E-3</v>
+        <v>92</v>
+      </c>
+      <c r="L33" s="2">
+        <v>3.5485968245378398E-2</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>716</v>
+        <v>404</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D34" s="1">
-        <v>28.1</v>
+        <v>10.9</v>
       </c>
       <c r="E34" s="1">
-        <v>34.200000000000003</v>
+        <v>14.5</v>
       </c>
       <c r="F34" s="1">
-        <v>36.9</v>
+        <v>23</v>
       </c>
       <c r="G34" s="1">
-        <v>40.462560000000003</v>
+        <v>23</v>
       </c>
       <c r="H34" s="4">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="I34" s="4">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="J34" s="4">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="K34" s="4">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="L34">
-        <v>-5.6679640415408801E-2</v>
+        <v>3.6270228264209101E-2</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>736</v>
+        <v>604</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="1">
+        <v>69</v>
+      </c>
+      <c r="E35" s="1">
+        <v>72.861500000000007</v>
+      </c>
+      <c r="F35" s="1">
+        <v>85</v>
+      </c>
+      <c r="G35" s="1">
+        <v>91.2</v>
+      </c>
+      <c r="H35" s="4">
+        <v>62</v>
+      </c>
+      <c r="I35" s="4">
+        <v>33</v>
+      </c>
+      <c r="J35" s="4">
+        <v>36</v>
+      </c>
+      <c r="K35" s="4">
         <v>34</v>
       </c>
-      <c r="D35" s="1">
-        <v>22.615659999999998</v>
-      </c>
-      <c r="E35" s="1">
-        <v>25.455850000000002</v>
-      </c>
-      <c r="F35" s="1">
-        <v>29</v>
-      </c>
-      <c r="G35" s="1">
-        <v>32.562559999999998</v>
-      </c>
-      <c r="H35" s="4">
-        <v>98</v>
-      </c>
-      <c r="I35" s="4">
-        <v>93</v>
-      </c>
-      <c r="J35" s="4">
-        <v>79</v>
-      </c>
-      <c r="K35" s="4">
-        <v>70</v>
-      </c>
       <c r="L35">
-        <v>-0.11851105026540799</v>
+        <v>6.3265690772740704E-2</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>748</v>
+        <v>231</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1">
-        <v>28.815660000000001</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1">
-        <v>31.655850000000001</v>
+        <v>12.7</v>
       </c>
       <c r="F36" s="1">
-        <v>35.200000000000003</v>
+        <v>23</v>
       </c>
       <c r="G36" s="1">
-        <v>42</v>
+        <v>26.562560000000001</v>
       </c>
       <c r="H36" s="4">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="I36" s="4">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="J36" s="4">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="K36" s="4">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="L36">
-        <v>1.17074193572516E-3</v>
+        <v>8.1858143841486306E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>760</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
-        <v>85.037729999999996</v>
+        <v>6.3377400000000002</v>
       </c>
       <c r="E37" s="1">
-        <v>86.6</v>
+        <v>6.7</v>
       </c>
       <c r="F37" s="1">
-        <v>92.7</v>
+        <v>15.2</v>
       </c>
       <c r="G37" s="1">
-        <v>96.262559999999993</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="H37" s="4">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="I37" s="4">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="J37" s="4">
-        <v>5</v>
+        <v>93</v>
       </c>
       <c r="K37" s="4">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="L37">
-        <v>-5.7549555396940698E-3</v>
+        <v>0.118656743469492</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2092,83 +2092,83 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>887</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>29</v>
+      </c>
+      <c r="E39" s="1">
+        <v>46.2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>49</v>
+      </c>
+      <c r="G39" s="1">
+        <v>53.7</v>
+      </c>
+      <c r="H39" s="4">
+        <v>94</v>
+      </c>
+      <c r="I39" s="4">
         <v>83</v>
       </c>
-      <c r="C39" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="1">
-        <v>38.459820000000001</v>
-      </c>
-      <c r="E39" s="1">
-        <v>41.3</v>
-      </c>
-      <c r="F39" s="1">
-        <v>44.8</v>
-      </c>
-      <c r="G39" s="1">
-        <v>48.406709999999997</v>
-      </c>
-      <c r="H39" s="4">
-        <v>48</v>
-      </c>
-      <c r="I39" s="4">
-        <v>39</v>
-      </c>
       <c r="J39" s="4">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="K39" s="4">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="L39">
-        <v>-3.6808169635344799E-2</v>
+        <v>0.29343089153145002</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>894</v>
+        <v>178</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D40" s="1">
-        <v>13.33774</v>
+        <v>24.387740000000001</v>
       </c>
       <c r="E40" s="1">
-        <v>17.399999999999999</v>
+        <v>20.9</v>
       </c>
       <c r="F40" s="1">
-        <v>18.5</v>
+        <v>37.1</v>
       </c>
       <c r="G40" s="1">
-        <v>22.062560000000001</v>
+        <v>41.6</v>
       </c>
       <c r="H40" s="4">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I40" s="4">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J40" s="4">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K40" s="4">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L40">
-        <v>-7.0376415114256297E-2</v>
+        <v>0.75270354476254997</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G41">
-    <sortCondition ref="A1"/>
+  <sortState ref="A2:L40">
+    <sortCondition ref="L1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>